<commit_message>
updated fullhalf cp_data map
</commit_message>
<xml_diff>
--- a/transcompiler/mapGenerators/maps/fulltohalf.xlsx
+++ b/transcompiler/mapGenerators/maps/fulltohalf.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="mWKrzVo6tkMb++6ytjy1oSfwDljGy5KOvgF9tLe4rpg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xr9L74jOMOtEPUuxdW2odNPIcnfk048Lfg94dadb6qw="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="836">
   <si>
     <t>FULL WIDTH</t>
   </si>
@@ -1951,6 +1951,25 @@
     <t>ﾟ</t>
   </si>
   <si>
+    <t>0x3099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBINING KATAKANA-HIRAGANA VOICED SOUND MARK
+</t>
+  </si>
+  <si>
+    <t>゙</t>
+  </si>
+  <si>
+    <t>0xFF9E</t>
+  </si>
+  <si>
+    <t>HALFWIDTH KATAKANA VOICED SOUND MARK</t>
+  </si>
+  <si>
+    <t>ﾞ</t>
+  </si>
+  <si>
     <t>0x309B</t>
   </si>
   <si>
@@ -1958,15 +1977,6 @@
   </si>
   <si>
     <t>゛</t>
-  </si>
-  <si>
-    <t>0xFF9E</t>
-  </si>
-  <si>
-    <t>HALFWIDTH KATAKANA VOICED SOUND MARK</t>
-  </si>
-  <si>
-    <t>ﾞ</t>
   </si>
   <si>
     <t>0x30FC</t>
@@ -2568,7 +2578,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2580,6 +2590,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -5604,16 +5620,14 @@
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="B109" s="3">
-        <v>12443.0</v>
-      </c>
-      <c r="C109" s="3" t="s">
+      <c r="B109" s="3"/>
+      <c r="C109" s="5" t="s">
         <v>645</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="6" t="s">
         <v>646</v>
       </c>
       <c r="F109" s="3" t="s">
@@ -5634,7 +5648,7 @@
         <v>650</v>
       </c>
       <c r="B110" s="3">
-        <v>12540.0</v>
+        <v>12443.0</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>651</v>
@@ -5643,265 +5657,290 @@
         <v>652</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="G110" s="3">
-        <v>65392.0</v>
+        <v>65438.0</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="I110" s="4" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B111" s="3">
+        <v>12540.0</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="F111" s="3" t="s">
         <v>656</v>
       </c>
-      <c r="B111" s="3">
+      <c r="G111" s="3">
+        <v>65392.0</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="I111" s="4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="A112" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="B112" s="3">
         <v>12539.0</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>657</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="G111" s="3">
+      <c r="C112" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="G112" s="3">
         <v>65381.0</v>
       </c>
-      <c r="H111" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="I111" s="4" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="D112" s="5" t="s">
+      <c r="H112" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="I112" s="4" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D113" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="F113" s="5" t="s">
+      <c r="F113" s="7" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="F114" s="5" t="s">
+      <c r="F114" s="7" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="F115" s="5" t="s">
+      <c r="F115" s="7" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D116" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="F116" s="5" t="s">
+      <c r="F116" s="7" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="F117" s="5" t="s">
+      <c r="F117" s="7" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="D118" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="F118" s="5" t="s">
+      <c r="F118" s="7" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="F119" s="5" t="s">
+      <c r="F119" s="7" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="F120" s="5" t="s">
+      <c r="F120" s="7" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="7" t="s">
         <v>689</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="F121" s="5" t="s">
+      <c r="F121" s="7" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="7" t="s">
         <v>692</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D122" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="F122" s="5" t="s">
+      <c r="F122" s="7" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D123" s="7" t="s">
         <v>696</v>
       </c>
-      <c r="F123" s="5" t="s">
+      <c r="F123" s="7" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="7" t="s">
         <v>698</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D124" s="7" t="s">
         <v>699</v>
       </c>
-      <c r="F124" s="5" t="s">
+      <c r="F124" s="7" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="7" t="s">
         <v>702</v>
       </c>
-      <c r="F125" s="5" t="s">
+      <c r="F125" s="7" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="7" t="s">
         <v>704</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="7" t="s">
         <v>705</v>
       </c>
-      <c r="F126" s="5" t="s">
+      <c r="F126" s="7" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="7" t="s">
         <v>707</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="7" t="s">
         <v>708</v>
       </c>
-      <c r="F127" s="5" t="s">
+      <c r="F127" s="7" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="D128" s="5" t="s">
+      <c r="D128" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="F128" s="5" t="s">
+      <c r="F128" s="7" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="7" t="s">
         <v>714</v>
       </c>
-      <c r="F129" s="5" t="s">
+      <c r="F129" s="7" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="7" t="s">
         <v>716</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130" s="7" t="s">
         <v>717</v>
       </c>
-      <c r="F130" s="5" t="s">
+      <c r="F130" s="7" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="7" t="s">
         <v>719</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="F131" s="5" t="s">
+      <c r="F131" s="7" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1">
+      <c r="A132" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>724</v>
+      </c>
+    </row>
     <row r="133" ht="15.75" customHeight="1"/>
     <row r="134" ht="15.75" customHeight="1"/>
     <row r="135" ht="15.75" customHeight="1"/>
@@ -6770,6 +6809,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
@@ -6814,534 +6854,534 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="B2" s="3">
         <v>12460.0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B3" s="3">
         <v>12462.0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B4" s="3">
         <v>12464.0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="B5" s="3">
         <v>12466.0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="B6" s="3">
         <v>12468.0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="B7" s="3">
         <v>12470.0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="B8" s="3">
         <v>12472.0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="B9" s="3">
         <v>12474.0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="B10" s="3">
         <v>12476.0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="B11" s="3">
         <v>12478.0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="B12" s="3">
         <v>12480.0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="B13" s="3">
         <v>12482.0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="B14" s="3">
         <v>12485.0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="B15" s="3">
         <v>12487.0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="B16" s="3">
         <v>12489.0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="B17" s="3">
         <v>12496.0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B18" s="3">
         <v>12497.0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="B19" s="3">
         <v>12499.0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="B20" s="3">
         <v>12500.0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="B21" s="3">
         <v>12502.0</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="B22" s="3">
         <v>12503.0</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="B23" s="3">
         <v>12505.0</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="B24" s="3">
         <v>12506.0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="B25" s="3">
         <v>12508.0</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="B26" s="3">
         <v>12509.0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="B27" s="3">
         <v>12526.0</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="B28" s="3">
         <v>12528.0</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="B29" s="3">
         <v>12529.0</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="B30" s="3">
         <v>12532.0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="B31" s="3">
         <v>12533.0</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="B32" s="3">
         <v>12534.0</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="B33" s="3">
         <v>12535.0</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="B34" s="3">
         <v>12536.0</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="B35" s="3">
         <v>12537.0</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="B36" s="3">
         <v>12538.0</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B37" s="3">
         <v>12540.0</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="B38" s="3">
         <v>12541.0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="B39" s="3">
         <v>12542.0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>

</xml_diff>